<commit_message>
del interpolated missing values from Co_L1
</commit_message>
<xml_diff>
--- a/volcanic_test/pincer_CO2/reaction_data.xlsx
+++ b/volcanic_test/pincer_CO2/reaction_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\pregabalin\RF\spectre\volcanic_test\pincer_CO2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\pregabalin\RF\spectre\volcanic_test\pincer_CO2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED72411-8364-4DB5-A4FD-8217836890ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CC2D1D-71F0-4AD7-94B0-B48CA276DFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{A82E05B1-9A49-4684-B31A-57BE8B7A83A2}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{A82E05B1-9A49-4684-B31A-57BE8B7A83A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -545,15 +543,15 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="8.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>47</v>
       </c>
@@ -603,7 +601,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -628,15 +626,11 @@
       <c r="H2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="I2" s="1">
-        <v>15</v>
-      </c>
+      <c r="I2" s="1"/>
       <c r="J2">
         <v>-0.9</v>
       </c>
-      <c r="K2" s="1">
-        <v>22</v>
-      </c>
+      <c r="K2" s="1"/>
       <c r="L2">
         <v>6.6</v>
       </c>
@@ -646,9 +640,7 @@
       <c r="N2">
         <v>-6.4</v>
       </c>
-      <c r="O2" s="1">
-        <v>32</v>
-      </c>
+      <c r="O2" s="1"/>
       <c r="P2">
         <v>-13.4</v>
       </c>
@@ -656,7 +648,7 @@
         <v>-39.9</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -703,7 +695,7 @@
         <v>-32.1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -747,7 +739,7 @@
         <v>-37.700000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -794,7 +786,7 @@
         <v>-42.2</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -841,7 +833,7 @@
         <v>-36.9</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -891,7 +883,7 @@
         <v>-37.6</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -938,7 +930,7 @@
         <v>-33.1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -982,7 +974,7 @@
         <v>-46.8</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1026,7 +1018,7 @@
         <v>-84.6</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1061,7 +1053,7 @@
         <v>-97.2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1099,7 +1091,7 @@
         <v>-99.4</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1140,7 +1132,7 @@
         <v>-91.4</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1181,7 +1173,7 @@
         <v>-82.8</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1219,7 +1211,7 @@
         <v>-89.7</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1263,7 +1255,7 @@
         <v>-93.9</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1298,7 +1290,7 @@
         <v>-82.9</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1345,7 +1337,7 @@
         <v>-90.9</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1383,7 +1375,7 @@
         <v>-85.2</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1421,7 +1413,7 @@
         <v>-87.9</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1465,7 +1457,7 @@
         <v>-130.30000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1503,7 +1495,7 @@
         <v>-148.69999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1541,7 +1533,7 @@
         <v>-148.4</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1582,7 +1574,7 @@
         <v>27.4</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1623,7 +1615,7 @@
         <v>37.299999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1667,7 +1659,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1705,7 +1697,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1740,7 +1732,7 @@
         <v>31.7</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1778,7 +1770,7 @@
         <v>35.9</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1822,7 +1814,7 @@
         <v>39.799999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1866,7 +1858,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1907,7 +1899,7 @@
         <v>-27.4</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1948,7 +1940,7 @@
         <v>-35.9</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>32</v>
       </c>

</xml_diff>